<commit_message>
Atualizando a ata e subindo o modelo da Calculadora de PERT
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/ATA-Semana 2A.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/ATA-Semana 2A.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpfer\OneDrive\Documentos\SPTECH\PI\SPRINT\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4fd29038e46714d/Área de Trabalho/SPTECH/Pesquisa e Inovação/Sprint-SPTECH/ATAs_de_Reuniao/Sprint 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39FD20B-E2AA-493D-B16F-24DF862ADF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{F39FD20B-E2AA-493D-B16F-24DF862ADF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACA3635E-1ADB-40DC-8B90-196B9021F1F9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="2" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Quinta" sheetId="1" r:id="rId1"/>
     <sheet name="Sexta" sheetId="3" r:id="rId2"/>
-    <sheet name="BANCO DE DADOS" sheetId="2" r:id="rId3"/>
+    <sheet name="Sábado" sheetId="4" r:id="rId3"/>
+    <sheet name="BANCO DE DADOS" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="39">
   <si>
     <t>NOME</t>
   </si>
@@ -149,6 +150,12 @@
   </si>
   <si>
     <t>Foi discutido sobre a alteração de data de prazos de entrega, junto da discussão, organização e preparo para a apresentação de TI no dia 25/09.</t>
+  </si>
+  <si>
+    <t>APRESENTAÇÃO DE TI</t>
+  </si>
+  <si>
+    <t>Ficou definida a parte de cada um dos integrantes na apresentação de TI: Introdução (Lucas Aiello), Ícones (Thiago), Diagrama (João Pedro e Lucas Pereira), Cálculo (Shelly) e Finalização (Miguel). Também combinamos uma data para treinarmos a apresentação pessoalente (Segunda-feira, 23/09).</t>
   </si>
 </sst>
 </file>
@@ -450,6 +457,9 @@
     <xf numFmtId="14" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -504,14 +514,161 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="54">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -763,103 +920,252 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1124,50 +1430,75 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F95CA63-C4C7-4EB6-955D-ED05E38937E0}" name="Tabela14" displayName="Tabela14" ref="A4:D12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F95CA63-C4C7-4EB6-955D-ED05E38937E0}" name="Tabela14" displayName="Tabela14" ref="A4:D12" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A7FACD00-2B31-4019-A56E-65C773E3AA49}" name="O QUE FAZER" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{9BDA6AAE-D8A7-451F-BDDB-C505248F0ED2}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{687F7861-FC98-4254-AEF3-B5108163FD30}" name="RESPONSAVEL" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{4CE5089F-14AC-4902-9804-474D2482620F}" name="SITUAÇÃO" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{A7FACD00-2B31-4019-A56E-65C773E3AA49}" name="O QUE FAZER" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{9BDA6AAE-D8A7-451F-BDDB-C505248F0ED2}" name="PRAZOS DE ENTREGA" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{687F7861-FC98-4254-AEF3-B5108163FD30}" name="RESPONSAVEL" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{4CE5089F-14AC-4902-9804-474D2482620F}" name="SITUAÇÃO" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{233261E1-B78E-4980-89B4-ECD8BA87118E}" name="Tabela25" displayName="Tabela25" ref="A21:C27" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{233261E1-B78E-4980-89B4-ECD8BA87118E}" name="Tabela25" displayName="Tabela25" ref="A21:C27" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BEAC01C6-9DF6-4F3E-AE22-4F43300E8D20}" name="NOME" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{22B38C5A-614F-40A6-9C22-AF72FFB3E3B6}" name="PARTICIPAÇÃO" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{571C9057-2775-4114-AC19-407CD64A10AE}" name="JUSTIFICATIVA" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{BEAC01C6-9DF6-4F3E-AE22-4F43300E8D20}" name="NOME" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{22B38C5A-614F-40A6-9C22-AF72FFB3E3B6}" name="PARTICIPAÇÃO" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{571C9057-2775-4114-AC19-407CD64A10AE}" name="JUSTIFICATIVA" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D24B965-B4D0-472F-8B6D-931251406FD0}" name="Tabela146" displayName="Tabela146" ref="A4:D11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
+  <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{4DB758E7-A5B8-4A9F-BCA4-563D8A6C3B6B}" name="O QUE FAZER" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{7EF6621B-1CC5-4635-882A-1B8E78882552}" name="PRAZOS DE ENTREGA" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{9F41E9D9-BCC0-44A3-9CEA-7746D12A0832}" name="RESPONSAVEL" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{C11A8EA2-A0AA-4B12-9B04-E8A9ADB179F1}" name="SITUAÇÃO" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{42551E1E-5CD7-4F6A-843E-1CBF547215BB}" name="Tabela257" displayName="Tabela257" ref="A20:C26" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+  <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8E8C9FBB-2737-4F1B-8662-DC7B8E05FE39}" name="NOME" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{5E83EC73-7E41-45E0-AF4D-68FC709F651A}" name="PARTICIPAÇÃO" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{87E32803-B844-4BA6-BF0A-17270B237D48}" name="JUSTIFICATIVA" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1496,38 +1827,38 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -1545,7 +1876,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1563,7 +1894,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1577,7 +1908,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1591,7 +1922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -1605,7 +1936,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -1619,7 +1950,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -1633,7 +1964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -1647,59 +1978,59 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
+    <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
-    </row>
-    <row r="18" spans="1:4" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -1713,7 +2044,7 @@
         <v>45554</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1725,7 +2056,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -1737,7 +2068,7 @@
         <v>0.68819444444444444</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -1749,7 +2080,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -1761,7 +2092,7 @@
         <v>0.69930555555555551</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -1773,7 +2104,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -1799,21 +2130,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D11">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1853,42 +2184,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30B5941-C936-4D38-8548-7C031F1187E9}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E16" activeCellId="1" sqref="E27 E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -1906,7 +2237,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1924,7 +2255,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1938,7 +2269,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1952,7 +2283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -1966,7 +2297,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -1980,7 +2311,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -1994,7 +2325,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -2008,59 +2339,59 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
+    <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-    </row>
-    <row r="17" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
-    </row>
-    <row r="18" spans="1:5" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-    </row>
-    <row r="19" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:5" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -2074,7 +2405,7 @@
         <v>45554</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -2086,7 +2417,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2098,7 +2429,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -2110,7 +2441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -2122,7 +2453,7 @@
         <v>0.70694444444444449</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -2134,7 +2465,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -2146,7 +2477,7 @@
         <f>IF(D25="","",D25-D23)</f>
         <v>1.2500000000000067E-2</v>
       </c>
-      <c r="E27" s="28"/>
+      <c r="E27" s="13"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -2158,21 +2489,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D11">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2209,6 +2540,347 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3CEB27-A829-4B68-B2D9-5D90AA774C8D}">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="46" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45556</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6">
+        <v>45559</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6">
+        <v>45556</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45559</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="6">
+        <v>45555</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="6">
+        <v>45558</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4">
+        <v>45556</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="7">
+        <v>0.41875000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="8">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="3">
+        <f>IF(D24="","",D24-D22)</f>
+        <v>6.2499999999999778E-3</v>
+      </c>
+      <c r="E26" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D17"/>
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B21:B26">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"AUSENTE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"PRESENTE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D10">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Finalizada"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Em Andamento"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Pendente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C11" xr:uid="{CF602ED2-C5AB-4338-A760-E49F25957E9B}">
+      <formula1>$A$21:$A$26</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{595204DC-DCAA-4657-89BE-3A3637AA945B}">
+          <x14:formula1>
+            <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B21:B26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{514D41D0-19FB-4FBD-8072-BB9890C483E1}">
+          <x14:formula1>
+            <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D5:D11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3E840F-4A34-4016-B525-4D6DE40DD748}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2216,12 +2888,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2232,7 +2904,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2243,7 +2915,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Animações finais no Slides PERT
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/ATA-Semana 2A.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/ATA-Semana 2A.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4fd29038e46714d/Área de Trabalho/SPTECH/Pesquisa e Inovação/Sprint-SPTECH/ATAs_de_Reuniao/Sprint 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Projeto_PI\sprint2\ATAs_de_Reuniao\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{F39FD20B-E2AA-493D-B16F-24DF862ADF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACA3635E-1ADB-40DC-8B90-196B9021F1F9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CA04C9-4FC4-43AF-9DC2-374CCDD30C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="2" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Quinta" sheetId="1" r:id="rId1"/>
     <sheet name="Sexta" sheetId="3" r:id="rId2"/>
     <sheet name="Sábado" sheetId="4" r:id="rId3"/>
-    <sheet name="BANCO DE DADOS" sheetId="2" r:id="rId4"/>
+    <sheet name="Segunda" sheetId="5" r:id="rId4"/>
+    <sheet name="BANCO DE DADOS" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="40">
   <si>
     <t>NOME</t>
   </si>
@@ -156,6 +157,9 @@
   </si>
   <si>
     <t>Ficou definida a parte de cada um dos integrantes na apresentação de TI: Introdução (Lucas Aiello), Ícones (Thiago), Diagrama (João Pedro e Lucas Pereira), Cálculo (Shelly) e Finalização (Miguel). Também combinamos uma data para treinarmos a apresentação pessoalente (Segunda-feira, 23/09).</t>
+  </si>
+  <si>
+    <t>Foi falado que iremos adiantar as tarefas ainda nesse dia e acelerar o processo de Sprint Review o quanto antes.</t>
   </si>
 </sst>
 </file>
@@ -518,157 +522,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="72">
     <dxf>
       <font>
         <b val="0"/>
@@ -920,6 +774,206 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1229,16 +1283,16 @@
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </left>
         <right style="medium">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </right>
         <top style="medium">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </top>
         <bottom style="medium">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
@@ -1254,7 +1308,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -1360,6 +1414,120 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1394,6 +1562,141 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1430,75 +1733,100 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" tableBorderDxfId="69">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F95CA63-C4C7-4EB6-955D-ED05E38937E0}" name="Tabela14" displayName="Tabela14" ref="A4:D12" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F95CA63-C4C7-4EB6-955D-ED05E38937E0}" name="Tabela14" displayName="Tabela14" ref="A4:D12" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A7FACD00-2B31-4019-A56E-65C773E3AA49}" name="O QUE FAZER" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{9BDA6AAE-D8A7-451F-BDDB-C505248F0ED2}" name="PRAZOS DE ENTREGA" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{687F7861-FC98-4254-AEF3-B5108163FD30}" name="RESPONSAVEL" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{4CE5089F-14AC-4902-9804-474D2482620F}" name="SITUAÇÃO" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{A7FACD00-2B31-4019-A56E-65C773E3AA49}" name="O QUE FAZER" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{9BDA6AAE-D8A7-451F-BDDB-C505248F0ED2}" name="PRAZOS DE ENTREGA" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{687F7861-FC98-4254-AEF3-B5108163FD30}" name="RESPONSAVEL" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{4CE5089F-14AC-4902-9804-474D2482620F}" name="SITUAÇÃO" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{233261E1-B78E-4980-89B4-ECD8BA87118E}" name="Tabela25" displayName="Tabela25" ref="A21:C27" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{233261E1-B78E-4980-89B4-ECD8BA87118E}" name="Tabela25" displayName="Tabela25" ref="A21:C27" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50" tableBorderDxfId="49">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BEAC01C6-9DF6-4F3E-AE22-4F43300E8D20}" name="NOME" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{22B38C5A-614F-40A6-9C22-AF72FFB3E3B6}" name="PARTICIPAÇÃO" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{571C9057-2775-4114-AC19-407CD64A10AE}" name="JUSTIFICATIVA" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{BEAC01C6-9DF6-4F3E-AE22-4F43300E8D20}" name="NOME" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{22B38C5A-614F-40A6-9C22-AF72FFB3E3B6}" name="PARTICIPAÇÃO" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{571C9057-2775-4114-AC19-407CD64A10AE}" name="JUSTIFICATIVA" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D24B965-B4D0-472F-8B6D-931251406FD0}" name="Tabela146" displayName="Tabela146" ref="A4:D11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D24B965-B4D0-472F-8B6D-931251406FD0}" name="Tabela146" displayName="Tabela146" ref="A4:D11" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4DB758E7-A5B8-4A9F-BCA4-563D8A6C3B6B}" name="O QUE FAZER" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{7EF6621B-1CC5-4635-882A-1B8E78882552}" name="PRAZOS DE ENTREGA" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{9F41E9D9-BCC0-44A3-9CEA-7746D12A0832}" name="RESPONSAVEL" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{C11A8EA2-A0AA-4B12-9B04-E8A9ADB179F1}" name="SITUAÇÃO" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{4DB758E7-A5B8-4A9F-BCA4-563D8A6C3B6B}" name="O QUE FAZER" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{7EF6621B-1CC5-4635-882A-1B8E78882552}" name="PRAZOS DE ENTREGA" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{9F41E9D9-BCC0-44A3-9CEA-7746D12A0832}" name="RESPONSAVEL" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{C11A8EA2-A0AA-4B12-9B04-E8A9ADB179F1}" name="SITUAÇÃO" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{42551E1E-5CD7-4F6A-843E-1CBF547215BB}" name="Tabela257" displayName="Tabela257" ref="A20:C26" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{42551E1E-5CD7-4F6A-843E-1CBF547215BB}" name="Tabela257" displayName="Tabela257" ref="A20:C26" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
   <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8E8C9FBB-2737-4F1B-8662-DC7B8E05FE39}" name="NOME" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{5E83EC73-7E41-45E0-AF4D-68FC709F651A}" name="PARTICIPAÇÃO" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{87E32803-B844-4BA6-BF0A-17270B237D48}" name="JUSTIFICATIVA" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{8E8C9FBB-2737-4F1B-8662-DC7B8E05FE39}" name="NOME" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{5E83EC73-7E41-45E0-AF4D-68FC709F651A}" name="PARTICIPAÇÃO" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{87E32803-B844-4BA6-BF0A-17270B237D48}" name="JUSTIFICATIVA" dataDxfId="33"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2973F3F9-B8D9-4E9E-BA21-0F7855C23630}" name="Tabela1468" displayName="Tabela1468" ref="A4:D11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{11646B81-A121-4FA2-893E-362D3A1A52F0}" name="O QUE FAZER" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{4833C381-32BB-4B40-AD0C-A01805D370D5}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{B9FED99E-7EE5-453D-998F-758D676F139A}" name="RESPONSAVEL" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{C9B39C91-0344-4E7A-847B-74EBED4B2F53}" name="SITUAÇÃO" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3C9D5C14-8487-4611-B27F-7F4ABC950782}" name="Tabela2579" displayName="Tabela2579" ref="A20:C26" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{66272961-D89D-4DD2-807F-D10CF138519D}" name="NOME" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{9700B9DF-18DC-4FF9-B87F-CA8E809DFE18}" name="PARTICIPAÇÃO" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{336A4CF9-2C48-4740-BBCF-05EBC653EB59}" name="JUSTIFICATIVA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2130,21 +2458,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D11">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2489,21 +2817,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D11">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2543,8 +2871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3CEB27-A829-4B68-B2D9-5D90AA774C8D}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="46" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" zoomScale="66" zoomScaleNormal="46" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2830,21 +3158,21 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="B21:B26">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2881,6 +3209,347 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02FDE50-A72F-4C17-8A91-E281A42AFC5E}">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="66" zoomScaleNormal="46" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45556</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6">
+        <v>45559</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6">
+        <v>45556</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45559</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="6">
+        <v>45555</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="6">
+        <v>45558</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4">
+        <v>45558</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="7">
+        <v>0.6958333333333333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="8">
+        <v>0.70138888888888884</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="3">
+        <f>IF(D24="","",D24-D22)</f>
+        <v>5.5555555555555358E-3</v>
+      </c>
+      <c r="E26" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D17"/>
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B21:B26">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+      <formula>"AUSENTE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+      <formula>"PRESENTE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D10">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+      <formula>"Finalizada"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+      <formula>"Em Andamento"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+      <formula>"Pendente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C11" xr:uid="{FAF4B15F-74B3-47F5-8B43-50363D8DED82}">
+      <formula1>$A$21:$A$26</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3CEAE7ED-D488-483E-8209-BAF021E091E9}">
+          <x14:formula1>
+            <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D5:D11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3856752-E5AE-441F-B371-26D903C39A26}">
+          <x14:formula1>
+            <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B21:B26</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3E840F-4A34-4016-B525-4D6DE40DD748}">
   <dimension ref="A1:D3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Adição da ata da daily do dia 24/02/2024
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/ATA-Semana 2A.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/ATA-Semana 2A.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Projeto_PI\sprint2\ATAs_de_Reuniao\Sprint 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPTech\GitHub\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CA04C9-4FC4-43AF-9DC2-374CCDD30C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F989479-9863-4E8B-8689-7A71FBF28E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Quinta" sheetId="1" r:id="rId1"/>
     <sheet name="Sexta" sheetId="3" r:id="rId2"/>
     <sheet name="Sábado" sheetId="4" r:id="rId3"/>
     <sheet name="Segunda" sheetId="5" r:id="rId4"/>
-    <sheet name="BANCO DE DADOS" sheetId="2" r:id="rId5"/>
+    <sheet name="Terça" sheetId="7" r:id="rId5"/>
+    <sheet name="BANCO DE DADOS" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="42">
   <si>
     <t>NOME</t>
   </si>
@@ -161,6 +162,12 @@
   <si>
     <t>Foi falado que iremos adiantar as tarefas ainda nesse dia e acelerar o processo de Sprint Review o quanto antes.</t>
   </si>
+  <si>
+    <t>Foi feito o treinamento da apresentação sobre a metodologia PERT</t>
+  </si>
+  <si>
+    <t>Apresentação na junta militar</t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,7 +529,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
+  <dxfs count="90">
     <dxf>
       <font>
         <b val="0"/>
@@ -693,7 +700,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -974,6 +981,56 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1142,7 +1199,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1391,7 +1448,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1532,16 +1589,16 @@
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </left>
         <right style="medium">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </right>
         <top style="medium">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </top>
         <bottom style="medium">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
@@ -1557,7 +1614,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -1640,7 +1697,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1663,6 +1720,120 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1697,6 +1868,141 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1733,100 +2039,125 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" tableBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" tableBorderDxfId="87">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="85"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="83"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5A356893-9A8B-4B13-8C28-51E182146249}" name="Tabela257911" displayName="Tabela257911" ref="A20:C26" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{139E8E28-282E-4954-A42E-FF13F888D8CB}" name="NOME" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{2D2F98D9-24BC-48E1-977F-50AADAAFFCD7}" name="PARTICIPAÇÃO" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{ECE86497-A781-4678-B780-5FE8694A399F}" name="JUSTIFICATIVA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81" tableBorderDxfId="80">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F95CA63-C4C7-4EB6-955D-ED05E38937E0}" name="Tabela14" displayName="Tabela14" ref="A4:D12" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F95CA63-C4C7-4EB6-955D-ED05E38937E0}" name="Tabela14" displayName="Tabela14" ref="A4:D12" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75" tableBorderDxfId="74">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A7FACD00-2B31-4019-A56E-65C773E3AA49}" name="O QUE FAZER" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{9BDA6AAE-D8A7-451F-BDDB-C505248F0ED2}" name="PRAZOS DE ENTREGA" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{687F7861-FC98-4254-AEF3-B5108163FD30}" name="RESPONSAVEL" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{4CE5089F-14AC-4902-9804-474D2482620F}" name="SITUAÇÃO" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{A7FACD00-2B31-4019-A56E-65C773E3AA49}" name="O QUE FAZER" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{9BDA6AAE-D8A7-451F-BDDB-C505248F0ED2}" name="PRAZOS DE ENTREGA" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{687F7861-FC98-4254-AEF3-B5108163FD30}" name="RESPONSAVEL" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{4CE5089F-14AC-4902-9804-474D2482620F}" name="SITUAÇÃO" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{233261E1-B78E-4980-89B4-ECD8BA87118E}" name="Tabela25" displayName="Tabela25" ref="A21:C27" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{233261E1-B78E-4980-89B4-ECD8BA87118E}" name="Tabela25" displayName="Tabela25" ref="A21:C27" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BEAC01C6-9DF6-4F3E-AE22-4F43300E8D20}" name="NOME" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{22B38C5A-614F-40A6-9C22-AF72FFB3E3B6}" name="PARTICIPAÇÃO" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{571C9057-2775-4114-AC19-407CD64A10AE}" name="JUSTIFICATIVA" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{BEAC01C6-9DF6-4F3E-AE22-4F43300E8D20}" name="NOME" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{22B38C5A-614F-40A6-9C22-AF72FFB3E3B6}" name="PARTICIPAÇÃO" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{571C9057-2775-4114-AC19-407CD64A10AE}" name="JUSTIFICATIVA" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D24B965-B4D0-472F-8B6D-931251406FD0}" name="Tabela146" displayName="Tabela146" ref="A4:D11" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D24B965-B4D0-472F-8B6D-931251406FD0}" name="Tabela146" displayName="Tabela146" ref="A4:D11" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
   <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4DB758E7-A5B8-4A9F-BCA4-563D8A6C3B6B}" name="O QUE FAZER" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{7EF6621B-1CC5-4635-882A-1B8E78882552}" name="PRAZOS DE ENTREGA" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{9F41E9D9-BCC0-44A3-9CEA-7746D12A0832}" name="RESPONSAVEL" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{C11A8EA2-A0AA-4B12-9B04-E8A9ADB179F1}" name="SITUAÇÃO" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{4DB758E7-A5B8-4A9F-BCA4-563D8A6C3B6B}" name="O QUE FAZER" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{7EF6621B-1CC5-4635-882A-1B8E78882552}" name="PRAZOS DE ENTREGA" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{9F41E9D9-BCC0-44A3-9CEA-7746D12A0832}" name="RESPONSAVEL" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{C11A8EA2-A0AA-4B12-9B04-E8A9ADB179F1}" name="SITUAÇÃO" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{42551E1E-5CD7-4F6A-843E-1CBF547215BB}" name="Tabela257" displayName="Tabela257" ref="A20:C26" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{42551E1E-5CD7-4F6A-843E-1CBF547215BB}" name="Tabela257" displayName="Tabela257" ref="A20:C26" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
   <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8E8C9FBB-2737-4F1B-8662-DC7B8E05FE39}" name="NOME" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{5E83EC73-7E41-45E0-AF4D-68FC709F651A}" name="PARTICIPAÇÃO" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{87E32803-B844-4BA6-BF0A-17270B237D48}" name="JUSTIFICATIVA" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{8E8C9FBB-2737-4F1B-8662-DC7B8E05FE39}" name="NOME" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{5E83EC73-7E41-45E0-AF4D-68FC709F651A}" name="PARTICIPAÇÃO" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{87E32803-B844-4BA6-BF0A-17270B237D48}" name="JUSTIFICATIVA" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2973F3F9-B8D9-4E9E-BA21-0F7855C23630}" name="Tabela1468" displayName="Tabela1468" ref="A4:D11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2973F3F9-B8D9-4E9E-BA21-0F7855C23630}" name="Tabela1468" displayName="Tabela1468" ref="A4:D11" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" tableBorderDxfId="48">
   <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{11646B81-A121-4FA2-893E-362D3A1A52F0}" name="O QUE FAZER" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{4833C381-32BB-4B40-AD0C-A01805D370D5}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{B9FED99E-7EE5-453D-998F-758D676F139A}" name="RESPONSAVEL" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{C9B39C91-0344-4E7A-847B-74EBED4B2F53}" name="SITUAÇÃO" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{11646B81-A121-4FA2-893E-362D3A1A52F0}" name="O QUE FAZER" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{4833C381-32BB-4B40-AD0C-A01805D370D5}" name="PRAZOS DE ENTREGA" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{B9FED99E-7EE5-453D-998F-758D676F139A}" name="RESPONSAVEL" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{C9B39C91-0344-4E7A-847B-74EBED4B2F53}" name="SITUAÇÃO" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3C9D5C14-8487-4611-B27F-7F4ABC950782}" name="Tabela2579" displayName="Tabela2579" ref="A20:C26" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3C9D5C14-8487-4611-B27F-7F4ABC950782}" name="Tabela2579" displayName="Tabela2579" ref="A20:C26" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
   <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{66272961-D89D-4DD2-807F-D10CF138519D}" name="NOME" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{9700B9DF-18DC-4FF9-B87F-CA8E809DFE18}" name="PARTICIPAÇÃO" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{336A4CF9-2C48-4740-BBCF-05EBC653EB59}" name="JUSTIFICATIVA" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{66272961-D89D-4DD2-807F-D10CF138519D}" name="NOME" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{9700B9DF-18DC-4FF9-B87F-CA8E809DFE18}" name="PARTICIPAÇÃO" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{336A4CF9-2C48-4740-BBCF-05EBC653EB59}" name="JUSTIFICATIVA" dataDxfId="38"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4239FFAB-7F81-4D5D-933C-45DFBF3605AD}" name="Tabela146810" displayName="Tabela146810" ref="A4:D11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{04C4A5A4-6229-4505-8F11-B7E824AC1473}" name="O QUE FAZER" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{E21C73CF-DFCA-4323-8C97-CBB757FA2560}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{9A31040F-148F-42BE-8FBC-5FCB2398EFB4}" name="RESPONSAVEL" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{4756F678-1E57-4686-8D68-E8BB92990CAB}" name="SITUAÇÃO" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2155,17 +2486,17 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
@@ -2173,8 +2504,8 @@
       <c r="C1" s="15"/>
       <c r="D1" s="16"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
@@ -2186,7 +2517,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -2204,7 +2535,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -2222,7 +2553,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -2236,7 +2567,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -2250,7 +2581,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -2264,7 +2595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -2278,7 +2609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -2292,7 +2623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -2306,14 +2637,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="17.45" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1"/>
+    <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -2321,7 +2652,7 @@
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1">
       <c r="A15" s="20" t="s">
         <v>35</v>
       </c>
@@ -2329,26 +2660,26 @@
       <c r="C15" s="21"/>
       <c r="D15" s="22"/>
     </row>
-    <row r="16" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="25"/>
     </row>
-    <row r="17" spans="1:4" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16.7" customHeight="1">
       <c r="A17" s="23"/>
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
       <c r="D17" s="25"/>
     </row>
-    <row r="18" spans="1:4" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="16.7" customHeight="1" thickBot="1">
       <c r="A18" s="26"/>
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
       <c r="D18" s="28"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1">
       <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
@@ -2358,7 +2689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -2372,7 +2703,7 @@
         <v>45554</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -2384,7 +2715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2396,7 +2727,7 @@
         <v>0.68819444444444444</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -2408,7 +2739,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -2420,7 +2751,7 @@
         <v>0.69930555555555551</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -2432,7 +2763,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -2458,21 +2789,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D11">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2516,17 +2847,17 @@
       <selection activeCell="E16" activeCellId="1" sqref="E27 E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
@@ -2534,8 +2865,8 @@
       <c r="C1" s="15"/>
       <c r="D1" s="16"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
@@ -2547,7 +2878,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -2565,7 +2896,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -2583,7 +2914,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -2597,7 +2928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -2611,7 +2942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -2625,7 +2956,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -2639,7 +2970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -2653,7 +2984,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -2667,14 +2998,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="17.45" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1"/>
+    <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -2682,7 +3013,7 @@
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1">
       <c r="A15" s="20" t="s">
         <v>36</v>
       </c>
@@ -2690,26 +3021,26 @@
       <c r="C15" s="21"/>
       <c r="D15" s="22"/>
     </row>
-    <row r="16" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="25"/>
     </row>
-    <row r="17" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="16.7" customHeight="1">
       <c r="A17" s="23"/>
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
       <c r="D17" s="25"/>
     </row>
-    <row r="18" spans="1:5" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="16.7" customHeight="1" thickBot="1">
       <c r="A18" s="26"/>
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
       <c r="D18" s="28"/>
     </row>
-    <row r="19" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" ht="6" customHeight="1" thickBot="1"/>
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1">
       <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
@@ -2719,7 +3050,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="24" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -2733,7 +3064,7 @@
         <v>45554</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -2745,7 +3076,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2757,7 +3088,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -2769,7 +3100,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -2781,7 +3112,7 @@
         <v>0.70694444444444449</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -2793,7 +3124,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -2817,21 +3148,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D11">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2875,17 +3206,17 @@
       <selection activeCell="A14" sqref="A14:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
@@ -2893,8 +3224,8 @@
       <c r="C1" s="15"/>
       <c r="D1" s="16"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
@@ -2906,7 +3237,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -2924,7 +3255,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -2938,7 +3269,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -2952,7 +3283,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
@@ -2966,7 +3297,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -2980,7 +3311,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -2994,7 +3325,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
@@ -3008,14 +3339,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1">
       <c r="A13" s="14" t="s">
         <v>34</v>
       </c>
@@ -3023,7 +3354,7 @@
       <c r="C13" s="15"/>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1">
       <c r="A14" s="20" t="s">
         <v>38</v>
       </c>
@@ -3031,26 +3362,26 @@
       <c r="C14" s="21"/>
       <c r="D14" s="22"/>
     </row>
-    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1">
       <c r="A15" s="23"/>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="25"/>
     </row>
-    <row r="16" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="25"/>
     </row>
-    <row r="17" spans="1:5" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="16.7" customHeight="1" thickBot="1">
       <c r="A17" s="26"/>
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="28"/>
     </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1">
       <c r="A19" s="17" t="s">
         <v>19</v>
       </c>
@@ -3060,7 +3391,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -3074,7 +3405,7 @@
         <v>45556</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3086,7 +3417,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -3098,7 +3429,7 @@
         <v>0.41875000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -3110,7 +3441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -3122,7 +3453,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -3134,7 +3465,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -3158,21 +3489,21 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="B21:B26">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3212,21 +3543,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02FDE50-A72F-4C17-8A91-E281A42AFC5E}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="66" zoomScaleNormal="46" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="66" zoomScaleNormal="46" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
@@ -3234,8 +3565,8 @@
       <c r="C1" s="15"/>
       <c r="D1" s="16"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
@@ -3247,7 +3578,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3265,7 +3596,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -3279,7 +3610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -3293,7 +3624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
@@ -3307,7 +3638,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -3321,7 +3652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -3335,7 +3666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
@@ -3349,14 +3680,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1">
       <c r="A13" s="14" t="s">
         <v>34</v>
       </c>
@@ -3364,7 +3695,7 @@
       <c r="C13" s="15"/>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1">
       <c r="A14" s="20" t="s">
         <v>39</v>
       </c>
@@ -3372,26 +3703,26 @@
       <c r="C14" s="21"/>
       <c r="D14" s="22"/>
     </row>
-    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1">
       <c r="A15" s="23"/>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="25"/>
     </row>
-    <row r="16" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="25"/>
     </row>
-    <row r="17" spans="1:5" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="16.7" customHeight="1" thickBot="1">
       <c r="A17" s="26"/>
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="28"/>
     </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1">
       <c r="A19" s="17" t="s">
         <v>19</v>
       </c>
@@ -3401,7 +3732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -3415,7 +3746,7 @@
         <v>45558</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3427,7 +3758,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -3439,7 +3770,7 @@
         <v>0.6958333333333333</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -3451,7 +3782,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -3463,7 +3794,7 @@
         <v>0.70138888888888884</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -3475,7 +3806,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -3499,21 +3830,21 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="B21:B26">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3550,6 +3881,349 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4FDFF8-372F-4860-BF40-AFBF460A6F78}">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="66" zoomScaleNormal="46" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1">
+      <c r="A1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1">
+      <c r="A3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9" ht="24" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:9" ht="17.45" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45556</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17.45" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6">
+        <v>45559</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17.45" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6">
+        <v>45556</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.45" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45559</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17.45" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="6">
+        <v>45555</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.45" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="6">
+        <v>45558</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.45" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1">
+      <c r="A13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.7" customHeight="1">
+      <c r="A14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.7" customHeight="1">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.7" customHeight="1">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.7" customHeight="1" thickBot="1">
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1">
+      <c r="A19" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1">
+      <c r="A20" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4">
+        <v>45559</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="7">
+        <v>0.68333333333333335</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
+      <c r="A23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
+      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="8">
+        <v>0.69444444444444442</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
+      <c r="A26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="3">
+        <f>IF(D24="","",D24-D22)</f>
+        <v>1.1111111111111072E-2</v>
+      </c>
+      <c r="E26" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D17"/>
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B21:B26">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+      <formula>"AUSENTE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+      <formula>"PRESENTE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D10">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+      <formula>"Finalizada"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+      <formula>"Em Andamento"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+      <formula>"Pendente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C11" xr:uid="{246F7448-B3F1-42C5-B8EC-A053A9779E64}">
+      <formula1>$A$21:$A$26</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D12E808-99D3-4425-8C97-AEE8CB7B788E}">
+          <x14:formula1>
+            <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B21:B26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6AD0849D-1BF5-420D-8141-480ABFF26CDB}">
+          <x14:formula1>
+            <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D5:D11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3E840F-4A34-4016-B525-4D6DE40DD748}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3557,12 +4231,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3573,7 +4247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3584,7 +4258,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>18</v>
       </c>

</xml_diff>